<commit_message>
EPBDS: updated demo application.
</commit_message>
<xml_diff>
--- a/DEMO/trunk/openl-bean-mapper-demo/src/main/resources/Chartis2AcordModelMappingExample.xlsx
+++ b/DEMO/trunk/openl-bean-mapper-demo/src/main/resources/Chartis2AcordModelMappingExample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Environment</t>
   </si>
@@ -105,34 +105,37 @@
     <t>Method String convertStringToC25(C25 source, String destination)</t>
   </si>
   <si>
-    <t>Method C4 convertIntToC4(int source, C4 destination)</t>
-  </si>
-  <si>
-    <t>Method int convertIntToC4(C4 source, int destination)</t>
-  </si>
-  <si>
     <t>convertIntToC4</t>
   </si>
   <si>
     <t>return Integer.valueOf(source.getId());</t>
   </si>
   <si>
+    <t xml:space="preserve">
+return source.getId();</t>
+  </si>
+  <si>
+    <t>org.openl.mapper.demo</t>
+  </si>
+  <si>
     <t>if (destination==null) {
-   destination = C25.Factory.newInstance();
+   destination = (C25)XmlBeanFactory.newInstance(C25.class);
 }
 destination.setId(source);
 return destination;</t>
   </si>
   <si>
-    <t xml:space="preserve">
-return source.getId();</t>
-  </si>
-  <si>
     <t>if (destination==null) {
-   destination = C4.Factory.newInstance();
+   destination = (C4)XmlBeanFactory.newInstance(C4.class);
 }
 destination.setId(String.valueOf(source));
 return destination;</t>
+  </si>
+  <si>
+    <t>Method C4 convertIntToC4(Integer source, C4 destination)</t>
+  </si>
+  <si>
+    <t>Method int convertIntToC4(C4 source, Integer destination)</t>
   </si>
 </sst>
 </file>
@@ -677,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -785,7 +788,7 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="3:9">
@@ -808,31 +811,31 @@
     </row>
     <row r="16" spans="3:9" ht="24" customHeight="1">
       <c r="C16" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D16" s="7"/>
     </row>
     <row r="19" spans="3:4">
       <c r="C19" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="3:4" ht="81.75" customHeight="1">
       <c r="C20" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="7"/>
     </row>
     <row r="22" spans="3:4">
       <c r="C22" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D23" s="7"/>
     </row>
@@ -867,10 +870,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C4:D7"/>
+  <dimension ref="C4:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -899,15 +902,21 @@
       </c>
     </row>
     <row r="7" spans="3:4">
-      <c r="C7" s="11"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4">
+      <c r="C8" s="11"/>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C5:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS: updated mapper demo
</commit_message>
<xml_diff>
--- a/DEMO/trunk/openl-bean-mapper-demo/src/main/resources/Chartis2AcordModelMappingExample.xlsx
+++ b/DEMO/trunk/openl-bean-mapper-demo/src/main/resources/Chartis2AcordModelMappingExample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Environment</t>
   </si>
@@ -72,15 +72,9 @@
     <t>policyNumber</t>
   </si>
   <si>
-    <t>persPolicy.policyNumber</t>
-  </si>
-  <si>
     <t>version</t>
   </si>
   <si>
-    <t>persPolicy.policyVersion</t>
-  </si>
-  <si>
     <t>com.exigen.chartis.integration.acord.pcsurety.generated</t>
   </si>
   <si>
@@ -94,12 +88,6 @@
   </si>
   <si>
     <t>Method String convertStringToC25(C25 source, String destination)</t>
-  </si>
-  <si>
-    <t>convertIntToC4</t>
-  </si>
-  <si>
-    <t>return Integer.valueOf(source.getId());</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -116,20 +104,34 @@
 return destination;</t>
   </si>
   <si>
-    <t>if (destination==null) {
-   destination = (C4)XmlBeanFactory.newInstance(C4.class);
-}
-destination.setId(String.valueOf(source));
-return destination;</t>
-  </si>
-  <si>
-    <t>Method C4 convertIntToC4(Integer source, C4 destination)</t>
-  </si>
-  <si>
-    <t>Method int convertIntToC4(C4 source, Integer destination)</t>
+    <t>persPolicy.policyVersion.stringValue</t>
+  </si>
+  <si>
+    <t>contractTerm.effective</t>
+  </si>
+  <si>
+    <t>contractTerm.expiration</t>
+  </si>
+  <si>
+    <t>persPolicy.contractTerm.effectiveDt.stringValue</t>
+  </si>
+  <si>
+    <t>persPolicy.contractTerm.expirationDt.stringValue</t>
+  </si>
+  <si>
+    <t>persPolicy.policyNumber</t>
   </si>
   <si>
     <t>convertStringToC25</t>
+  </si>
+  <si>
+    <t>producerCd</t>
+  </si>
+  <si>
+    <t>producerArray[0].producerInfo.contractNumber.stringValue</t>
+  </si>
+  <si>
+    <t>producerArray[1].producerInfo.contractNumber.stringValue</t>
   </si>
 </sst>
 </file>
@@ -672,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C3:H22"/>
+  <dimension ref="C3:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -740,97 +742,96 @@
     </row>
     <row r="6" spans="3:8">
       <c r="C6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="3:8">
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8">
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
-        <v>26</v>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="3:8">
-      <c r="C11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="3:8" ht="80.25" customHeight="1">
-      <c r="C12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="14" spans="3:8">
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="3:8" ht="24" customHeight="1">
-      <c r="C15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="18" spans="3:4">
-      <c r="C18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="3:4" ht="81.75" customHeight="1">
-      <c r="C19" s="6" t="s">
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="21" spans="3:4">
-      <c r="C21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="3:4">
-      <c r="C22" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="7"/>
-    </row>
+    </row>
+    <row r="12" spans="3:8">
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8">
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="80.25" customHeight="1"/>
+    <row r="17" ht="24" customHeight="1"/>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
+  <mergeCells count="1">
     <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -839,12 +840,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B3:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="2:3" ht="99.75" customHeight="1">
+      <c r="B4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="2:3" ht="24.75" customHeight="1">
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -879,7 +916,7 @@
     <row r="6" spans="3:4">
       <c r="C6" s="10"/>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="3:4">
@@ -891,7 +928,7 @@
     <row r="8" spans="3:4">
       <c r="C8" s="11"/>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>